<commit_message>
read registers, begin ALU
</commit_message>
<xml_diff>
--- a/MIPSCel.xlsx
+++ b/MIPSCel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cooperterrill/Desktop/MIPCel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525C6054-13D4-1F44-9F44-46C62E603AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691D5A3A-DAFA-3245-BF9C-D2E6E8AF7E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19300" xr2:uid="{95E4A03E-3FED-BF42-ACD2-5D2E65B33E92}"/>
   </bookViews>
@@ -16,29 +16,29 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="a">Sheet1!$E$51:$H$51</definedName>
-    <definedName name="b">Sheet1!$E$52:$H$52</definedName>
-    <definedName name="c_">Sheet1!$E$53:$H$53</definedName>
     <definedName name="CLK">Sheet1!$A$200</definedName>
     <definedName name="CLR">Sheet1!$B$200</definedName>
-    <definedName name="d">Sheet1!$E$54:$H$54</definedName>
-    <definedName name="Format_I">Sheet1!$F$36:$J$36</definedName>
+    <definedName name="FNCT">Sheet1!$D$31</definedName>
     <definedName name="IFMT">Sheet1!$E$37</definedName>
-    <definedName name="Imd">Sheet1!$F$31:$J$31</definedName>
+    <definedName name="IMMD">Sheet1!$F$31</definedName>
     <definedName name="INSTR">Sheet1!$A$36</definedName>
+    <definedName name="JADDR">Sheet1!$H$31</definedName>
     <definedName name="JFMT">Sheet1!$G$37</definedName>
     <definedName name="OP">Sheet1!$B$36</definedName>
-    <definedName name="OP1_">Sheet1!$F$13:$J$13</definedName>
-    <definedName name="PC">Sheet1!$J$7</definedName>
-    <definedName name="Q">Sheet1!$F$19:$J$19</definedName>
+    <definedName name="PC">Sheet1!$G$7</definedName>
+    <definedName name="RD">Sheet1!$D$33</definedName>
+    <definedName name="RDADDR">Sheet1!$D$26</definedName>
     <definedName name="RFMT">Sheet1!$C$37</definedName>
-    <definedName name="s1_">Sheet1!$F$6:$J$6</definedName>
-    <definedName name="T_flip_flop">Sheet1!$F$17:$J$17</definedName>
-    <definedName name="t3_">Sheet1!$F$4:$J$4</definedName>
-    <definedName name="t9_">Sheet1!$F$8:$J$8</definedName>
-    <definedName name="v1_">Sheet1!$F$2:$J$2</definedName>
+    <definedName name="RS">Sheet1!$D$35</definedName>
+    <definedName name="RSADDR">Sheet1!$D$28</definedName>
+    <definedName name="RSVAL">Sheet1!$D$23</definedName>
+    <definedName name="RT">Sheet1!$D$34</definedName>
+    <definedName name="RTADDR">Sheet1!$D$27</definedName>
+    <definedName name="RTVAL">Sheet1!$D$22</definedName>
+    <definedName name="SHMT">Sheet1!$D$32</definedName>
   </definedNames>
-  <calcPr calcId="181029" refMode="R1C1" iterate="1" iterateDelta="1E+16" calcOnSave="0" forceFullCalc="1"/>
+  <calcPr calcId="191029" calcMode="manual" refMode="R1C1" iterate="1" iterateDelta="1E+16" calcCompleted="0" calcOnSave="0" forceFullCalc="1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,19 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
-  <si>
-    <t>Adder</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>D-flip flop</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>SOURCE</t>
   </si>
@@ -120,9 +108,6 @@
   </si>
   <si>
     <t>CLR</t>
-  </si>
-  <si>
-    <t>T-flip flop</t>
   </si>
   <si>
     <t>v0</t>
@@ -227,34 +212,7 @@
     <t>Format=J</t>
   </si>
   <si>
-    <t>Rs</t>
-  </si>
-  <si>
-    <t>Rt</t>
-  </si>
-  <si>
-    <t>Rd</t>
-  </si>
-  <si>
-    <t>Shamt</t>
-  </si>
-  <si>
-    <t>Funct</t>
-  </si>
-  <si>
-    <t>Imd</t>
-  </si>
-  <si>
-    <t>Addr</t>
-  </si>
-  <si>
     <t>pc</t>
-  </si>
-  <si>
-    <t>OP1</t>
-  </si>
-  <si>
-    <t>OP2</t>
   </si>
   <si>
     <t>128x128</t>
@@ -295,12 +253,66 @@
   <si>
     <t>SUC?</t>
   </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>RSADDR</t>
+  </si>
+  <si>
+    <t>RTADDR</t>
+  </si>
+  <si>
+    <t>JADDR</t>
+  </si>
+  <si>
+    <t>IMMD</t>
+  </si>
+  <si>
+    <t>FNCT</t>
+  </si>
+  <si>
+    <t>SHMT</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>RDADDR</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>done:</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>case:</t>
+  </si>
+  <si>
+    <t>0/32</t>
+  </si>
+  <si>
+    <t>RTVAL</t>
+  </si>
+  <si>
+    <t>RSVAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,12 +324,6 @@
       <sz val="13"/>
       <color rgb="FF0C0D0E"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -717,159 +723,155 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:DX201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="132" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
+      <c r="N2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3">
         <f ca="1">CLK</f>
         <v>0</v>
       </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J7">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
       <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <f ca="1">RTVAL+RSVAL</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F14">
-        <f>E14+G14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -877,88 +879,119 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <f ca="1">IF(CLR = 1, 0, $A$20 + 1)</f>
-        <v>1364</v>
+        <v>1410</v>
       </c>
-      <c r="D20">
-        <f ca="1">IF(CLK = 1, $A$20,$D$20)</f>
-        <v>1363</v>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>67</v>
       </c>
-      <c r="E20" t="b">
-        <f ca="1">IF(MOD($A$20,7) = 0, NOT($E$20), $E$20)</f>
+      <c r="D22" cm="1">
+        <f t="array" aca="1" ref="D22" ca="1">INDIRECT(RTADDR)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">INDIRECT(RSADDR)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" t="str">
+        <f ca="1">IF(RFMT,ADDRESS(_xlfn.BITRSHIFT(RD,3)*2 + 1, 1+_xlfn.BITAND(RD,7)),RDADDR)</f>
+        <v>$D$3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="str">
+        <f ca="1">IF(RFMT,ADDRESS(_xlfn.BITRSHIFT(RT,3)*2 + 1, 1+_xlfn.BITAND(RT,7)),RTADDR)</f>
+        <v>$F$3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="str">
+        <f ca="1">IF(RFMT,ADDRESS(_xlfn.BITRSHIFT(RS,3)*2 + 1, 1+_xlfn.BITAND(RS,7)),RSADDR)</f>
+        <v>$H$3</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D31">
-        <f>IF(RFMT, _xlfn.BITAND(INSTR,127),$D$31)</f>
+        <f ca="1">IF(RFMT, _xlfn.BITAND(INSTR,127),$D$31)</f>
         <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F31">
-        <f ca="1">IF(IFMT,_xlfn.BITAND(INSTR,65535),$F$31)</f>
-        <v>15</v>
+        <f ca="1">IF(IFMT,_xlfn.BITAND(INSTR,65535),IMMD)</f>
+        <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
-      <c r="H31" t="b">
-        <f>IF(JFMT,_xlfn.BITAND(INSTR,134217727))</f>
+      <c r="H31">
+        <f ca="1">IF(JFMT,_xlfn.BITAND(INSTR,134217727),JADDR)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D32">
-        <f>IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,6),31),$D$32)</f>
+        <f ca="1">IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,6),31),$D$32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D33">
-        <f>IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,11),31),$D$33)</f>
+        <f ca="1">IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,11),31),$D$33)</f>
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D34">
-        <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,16),31),$D$34)</f>
+        <f ca="1">IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,16),31),$D$34)</f>
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D35">
-        <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),$D$35)</f>
+        <f ca="1">IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),$D$35)</f>
         <v>15</v>
       </c>
     </row>
@@ -971,88 +1004,88 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G36" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C37" t="b">
-        <f>(OP=0)</f>
+        <f ca="1">(OP=0)</f>
         <v>1</v>
       </c>
       <c r="E37" t="b">
-        <f>AND(NOT(RFMT),NOT(JFMT))</f>
+        <f ca="1">AND(NOT(RFMT),NOT(JFMT))</f>
         <v>0</v>
       </c>
       <c r="G37" t="b">
-        <f>OR(OP=2,OP=3,OP=26)</f>
+        <f ca="1">OR(OP=2,OP=3,OP=26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M43" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G45" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H45" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="L45" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="M45" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="N45" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="O45" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G46">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H46" t="str">
         <f>ADDRESS(_xlfn.BITRSHIFT($G$46,6)+50,1+_xlfn.BITAND($G$46,127))</f>
-        <v>$O$50</v>
+        <v>$E$50</v>
       </c>
-      <c r="I46" cm="1">
+      <c r="I46" t="str" cm="1">
         <f t="array" aca="1" ref="I46" ca="1">INDIRECT($H$46)</f>
-        <v>0</v>
+        <v>pen</v>
       </c>
       <c r="L46">
         <v>12</v>
@@ -1064,22 +1097,22 @@
       <c r="N46">
         <v>34</v>
       </c>
-      <c r="O46" cm="1">
+      <c r="O46" t="e" cm="1">
         <f t="array" aca="1" ref="O46" ca="1">SetCellValue(CELL("contents",$M$46),$N$46)</f>
-        <v>1</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:128" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f>ADDRESS(_xlfn.BITRSHIFT(PC,6)+50,1+_xlfn.BITAND(PC,127))</f>
+        <f ca="1">ADDRESS(_xlfn.BITRSHIFT(PC,6)+50,1+_xlfn.BITAND(PC,127))</f>
         <v>$D$50</v>
       </c>
       <c r="B49" t="str" cm="1">
@@ -1092,9 +1125,11 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -1224,7 +1259,7 @@
     <row r="51" spans="1:128" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -17874,10 +17909,10 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add support for some i/j format instructions
</commit_message>
<xml_diff>
--- a/MIPSCel.xlsx
+++ b/MIPSCel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cooperterrill/Desktop/MIPCel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB57B34-1BA9-6D49-B4C9-383EDB900E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934F094-7F91-5347-9957-B27F44884266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="17100" windowHeight="19300" xr2:uid="{95E4A03E-3FED-BF42-ACD2-5D2E65B33E92}"/>
   </bookViews>
@@ -24,9 +24,10 @@
     <definedName name="INSTR">Sheet1!$A$36</definedName>
     <definedName name="JBITS">Sheet1!$H$31</definedName>
     <definedName name="JFMT">Sheet1!$G$37</definedName>
-    <definedName name="LWBASE">Sheet1!$F$26</definedName>
+    <definedName name="LWBASE">Sheet1!$F$27</definedName>
+    <definedName name="LWBASEADDR">Sheet1!$F$26</definedName>
     <definedName name="OP">Sheet1!$B$36</definedName>
-    <definedName name="PC">Sheet1!$G$7</definedName>
+    <definedName name="PC">Sheet1!$H$7</definedName>
     <definedName name="RD">Sheet1!$D$33</definedName>
     <definedName name="RDADDR">Sheet1!$D$26</definedName>
     <definedName name="RFMT">Sheet1!$C$37</definedName>
@@ -66,6 +67,7 @@
     <author>tc={1B919823-7042-AA45-8BE7-2E148AF7736E}</author>
     <author>tc={CDCDC5D9-ED0E-2148-BF8A-9DA016F77D57}</author>
     <author>tc={76E4CB42-0AD5-5B4D-A6A1-B3EAB175ADCF}</author>
+    <author>tc={9C796C1D-7C14-8143-A65D-F6D2F20500E3}</author>
     <author>tc={0A142261-3ADA-D24A-85B9-D6D70B5D60C5}</author>
     <author>tc={669385F9-156F-9D40-9551-F4A1471536C0}</author>
   </authors>
@@ -125,10 +127,20 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Should the offset be indexed like this?</t>
+    Should the offset be indexed like this?
+Reply:
+    Rn it’s value at register pointed to by lwbaseaddr + IMMD. So either can be not word-aligned, but sum MUST be word-aligned so I don’t shit myself</t>
       </text>
     </comment>
-    <comment ref="C27" authorId="4" shapeId="0" xr:uid="{0A142261-3ADA-D24A-85B9-D6D70B5D60C5}">
+    <comment ref="E26" authorId="4" shapeId="0" xr:uid="{9C796C1D-7C14-8143-A65D-F6D2F20500E3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Might make conditional</t>
+      </text>
+    </comment>
+    <comment ref="C27" authorId="5" shapeId="0" xr:uid="{0A142261-3ADA-D24A-85B9-D6D70B5D60C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -136,7 +148,7 @@
     Same</t>
       </text>
     </comment>
-    <comment ref="C28" authorId="5" shapeId="0" xr:uid="{669385F9-156F-9D40-9551-F4A1471536C0}">
+    <comment ref="C28" authorId="6" shapeId="0" xr:uid="{669385F9-156F-9D40-9551-F4A1471536C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -171,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>SOURCE</t>
   </si>
@@ -453,6 +465,12 @@
   </si>
   <si>
     <t>LWBASE</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>LWBASEADDR</t>
   </si>
 </sst>
 </file>
@@ -881,6 +899,12 @@
   <threadedComment ref="G22" dT="2024-05-18T05:40:00.35" personId="{91AC9A71-FD55-054C-B785-052ED73AB046}" id="{76E4CB42-0AD5-5B4D-A6A1-B3EAB175ADCF}">
     <text>Should the offset be indexed like this?</text>
   </threadedComment>
+  <threadedComment ref="G22" dT="2024-05-18T06:01:12.30" personId="{91AC9A71-FD55-054C-B785-052ED73AB046}" id="{8548F688-C553-7749-92C9-E7471DADE7A4}" parentId="{76E4CB42-0AD5-5B4D-A6A1-B3EAB175ADCF}">
+    <text>Rn it’s value at register pointed to by lwbaseaddr + IMMD. So either can be not word-aligned, but sum MUST be word-aligned so I don’t shit myself</text>
+  </threadedComment>
+  <threadedComment ref="E26" dT="2024-05-18T05:58:40.63" personId="{91AC9A71-FD55-054C-B785-052ED73AB046}" id="{9C796C1D-7C14-8143-A65D-F6D2F20500E3}">
+    <text>Might make conditional</text>
+  </threadedComment>
   <threadedComment ref="C27" dT="2024-05-18T05:44:13.32" personId="{91AC9A71-FD55-054C-B785-052ED73AB046}" id="{0A142261-3ADA-D24A-85B9-D6D70B5D60C5}">
     <text>Same</text>
   </threadedComment>
@@ -893,10 +917,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5337B1-3AE4-EB42-9D14-4ACDB1D87C75}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:DX201"/>
+  <dimension ref="A1:DX201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="132" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,30 +932,35 @@
     <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
       <c r="N2" t="s">
         <v>1</v>
@@ -940,86 +969,89 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N3">
         <f ca="1">CLK</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G7">
+      <c r="H7">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1197,7 +1229,7 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <f ca="1">IF(CLR = 1, 0, $A$20 + 1)</f>
-        <v>1429</v>
+        <v>1438</v>
       </c>
       <c r="G20" t="s">
         <v>90</v>
@@ -1205,6 +1237,9 @@
       <c r="H20">
         <f ca="1">IF(RSVAL=RTVAL,_xlfn.BITLSHIFT(IMMD,2)+PC+4,PC+4)</f>
         <v>44</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1214,6 +1249,9 @@
       <c r="H21">
         <f ca="1">IF(RSVAL&lt;&gt;RTVAL,_xlfn.BITLSHIFT(IMMD,2)+PC+4,PC+4)</f>
         <v>12</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -1227,9 +1265,12 @@
       <c r="G22" t="s">
         <v>92</v>
       </c>
-      <c r="H22">
-        <f>LWBASE+_xlfn.BITLSHIFT(IMMD,4)</f>
-        <v>139</v>
+      <c r="H22" cm="1">
+        <f t="array" aca="1" ref="H22" ca="1">INDIRECT(LWBASEADDR)+IMMD</f>
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -1246,15 +1287,15 @@
         <v>60</v>
       </c>
       <c r="D26" t="str">
-        <f ca="1">IF(RFMT,ADDRESS(_xlfn.BITRSHIFT(RD,3)*2 + 1, 1+_xlfn.BITAND(RD,7)),RDADDR)</f>
-        <v>$D$3</v>
+        <f>IF(RFMT,ADDRESS(_xlfn.BITRSHIFT(RD,3)*2 + 1, 1+_xlfn.BITAND(RD,7)),RDADDR)</f>
+        <v>$C$1</v>
       </c>
       <c r="E26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
-      <c r="F26">
-        <f>IF(OP=35,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),LWBASE)</f>
-        <v>11</v>
+      <c r="F26" t="str">
+        <f ca="1">ADDRESS(_xlfn.BITRSHIFT(LWBASE,3)*2 + 1, 1+_xlfn.BITAND(LWBASE,7))</f>
+        <v>$F$1</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -1263,7 +1304,14 @@
       </c>
       <c r="D27" t="str">
         <f>ADDRESS(_xlfn.BITRSHIFT(RT,3)*2 + 1, 1+_xlfn.BITAND(RT,7))</f>
-        <v>$B$3</v>
+        <v>$D$3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27">
+        <f ca="1">IF(OP=35,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),LWBASE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -1272,7 +1320,7 @@
       </c>
       <c r="D28" t="str">
         <f>ADDRESS(_xlfn.BITRSHIFT(RS,3)*2 + 1, 1+_xlfn.BITAND(RS,7))</f>
-        <v>$D$3</v>
+        <v>$H$1</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -1280,14 +1328,14 @@
         <v>55</v>
       </c>
       <c r="D31">
-        <f ca="1">IF(RFMT, _xlfn.BITAND(INSTR,127),$D$31)</f>
+        <f>IF(RFMT, _xlfn.BITAND(INSTR,127),$D$31)</f>
         <v>32</v>
       </c>
       <c r="E31" t="s">
         <v>54</v>
       </c>
       <c r="F31">
-        <f>IF(IFMT,_xlfn.BITAND(INSTR,65535),IMMD)</f>
+        <f ca="1">IF(IFMT,_xlfn.BITAND(INSTR,65535),IMMD)</f>
         <v>8</v>
       </c>
       <c r="G31" t="s">
@@ -1303,7 +1351,7 @@
         <v>56</v>
       </c>
       <c r="D32">
-        <f ca="1">IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,6),31),$D$32)</f>
+        <f>IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,6),31),$D$32)</f>
         <v>0</v>
       </c>
     </row>
@@ -1312,8 +1360,8 @@
         <v>57</v>
       </c>
       <c r="D33">
-        <f ca="1">IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,11),31),$D$33)</f>
-        <v>11</v>
+        <f>IF(RFMT,_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,11),31),$D$33)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -1322,7 +1370,7 @@
       </c>
       <c r="D34">
         <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,16),31),$D$34)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1331,16 +1379,16 @@
       </c>
       <c r="D35">
         <f>IF(OR(RFMT,IFMT),_xlfn.BITAND(_xlfn.BITRSHIFT(INSTR,21),31),$D$35)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2372468744</v>
+        <v>15405088</v>
       </c>
       <c r="B36">
         <f>_xlfn.BITRSHIFT($A$36,26)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -1361,11 +1409,11 @@
       </c>
       <c r="C37" t="b">
         <f>(OP=0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="b">
         <f>AND(NOT(RFMT),NOT(JFMT))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="b">
         <f>OR(OP=2,OP=3,OP=26)</f>
@@ -18240,7 +18288,7 @@
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <f ca="1">IF($A$200 = 1,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B200" s="2">
         <v>0</v>

</xml_diff>